<commit_message>
Updated other models and created Microsoft DCF model
</commit_message>
<xml_diff>
--- a/AMD DCF 10-26-22.xlsx
+++ b/AMD DCF 10-26-22.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bina/Documents/financial-modeling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADF10C5A-8173-4045-BA2A-0F653EC46B9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E040C85-2BB8-984C-A9B8-37EBEA9D5788}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="23860" yWindow="460" windowWidth="27120" windowHeight="26980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1135" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1136" uniqueCount="136">
   <si>
     <t>INCOME STATEMENT (in mln.)</t>
   </si>
@@ -438,6 +438,9 @@
   </si>
   <si>
     <t>Upside / Downside</t>
+  </si>
+  <si>
+    <t>Present Value of Future Cash Flows</t>
   </si>
 </sst>
 </file>
@@ -650,7 +653,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -759,6 +762,9 @@
     </xf>
     <xf numFmtId="9" fontId="15" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1081,7 +1087,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="AH68" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="AK88" sqref="AK88"/>
+      <selection pane="bottomRight" activeCell="A101" sqref="A101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13053,7 +13059,9 @@
       </c>
     </row>
     <row r="101" spans="1:42" ht="19" x14ac:dyDescent="0.25">
-      <c r="A101" s="5"/>
+      <c r="A101" s="53" t="s">
+        <v>135</v>
+      </c>
       <c r="B101" s="13"/>
       <c r="C101" s="13"/>
       <c r="D101" s="13"/>
@@ -13169,7 +13177,7 @@
       <c r="AL110" s="48"/>
       <c r="AM110" s="49"/>
     </row>
-    <row r="111" spans="1:42" ht="34" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:42" ht="17" x14ac:dyDescent="0.2">
       <c r="AL111" s="50" t="s">
         <v>133</v>
       </c>
@@ -13178,7 +13186,7 @@
         <v>SELL</v>
       </c>
     </row>
-    <row r="112" spans="1:42" ht="34" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:42" ht="17" x14ac:dyDescent="0.2">
       <c r="AL112" s="50" t="s">
         <v>134</v>
       </c>

</xml_diff>